<commit_message>
Restructured project, added model evaluation
</commit_message>
<xml_diff>
--- a/data/fight_card.xlsx
+++ b/data/fight_card.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1572750901" val="971" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1572750901" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1572750901"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1572750901"/>
+      <pm:revision xmlns:pm="smNativeData" day="1596287657" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1596287657" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1596287657" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1596287657"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>weight_class</t>
   </si>
@@ -34,13 +34,40 @@
     <t>fighter2</t>
   </si>
   <si>
+    <t>Middleweight</t>
+  </si>
+  <si>
+    <t>Edmen Shahbazyan</t>
+  </si>
+  <si>
+    <t>Derek Brunson</t>
+  </si>
+  <si>
+    <t>Women's Flyweight</t>
+  </si>
+  <si>
+    <t>Jennifer Maia</t>
+  </si>
+  <si>
+    <t>Joanne Calderwood</t>
+  </si>
+  <si>
     <t>Welterweight</t>
   </si>
   <si>
-    <t>Stephen Thompson</t>
+    <t>Randy Brown</t>
   </si>
   <si>
     <t>Vicente Luque</t>
+  </si>
+  <si>
+    <t>Lightweight</t>
+  </si>
+  <si>
+    <t>Justin Gaethje</t>
+  </si>
+  <si>
+    <t>Khabib Nurmagomedov</t>
   </si>
 </sst>
 </file>
@@ -65,7 +92,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1572750901" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1596287657" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -74,26 +101,15 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1572750901" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -109,26 +125,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572750901"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1572750901"/>
+          <pm:border xmlns:pm="smNativeData" id="1596287657"/>
         </ext>
       </extLst>
     </border>
@@ -145,7 +142,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1572750901" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1596287657" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -409,10 +406,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="B1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -434,10 +431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="n">
-        <v>8</v>
-      </c>
+    <row r="2" spans="2:5">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -447,12 +441,49 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2"/>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4"/>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5"/>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1572750901" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1596287657" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -461,16 +492,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1572750901" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1572750901" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1572750901" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1572750901" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1596287657" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1596287657" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1596287657" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1596287657" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1572750901" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1596287657" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>